<commit_message>
change: added IC in vendor upload
</commit_message>
<xml_diff>
--- a/assets/templates/vendor_upload_template.xlsx
+++ b/assets/templates/vendor_upload_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Libra\Backend\assets\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Libra\System\latest\rata_backend\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6C74D9-3EDC-489F-8453-4DA8C213A4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7151837A-E0ED-45E2-9407-2C57D3E2CA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Zip Code</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>ASCII Vendor Code</t>
+  </si>
+  <si>
+    <t>is_ic</t>
+  </si>
+  <si>
+    <t>Is IC?</t>
   </si>
 </sst>
 </file>
@@ -428,21 +434,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -476,8 +483,11 @@
       <c r="K1" t="s">
         <v>26</v>
       </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -510,6 +520,9 @@
       </c>
       <c r="K2" t="s">
         <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>